<commit_message>
Final product backlog commit
</commit_message>
<xml_diff>
--- a/Product_Backlog/ProductBacklogDay5.xlsx
+++ b/Product_Backlog/ProductBacklogDay5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruthc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1019A8D4-8D34-4611-9C20-305B49F5ACE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75207597-B66C-4C6D-B223-A09ED7E28E27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t>As an....</t>
   </si>
@@ -113,9 +113,6 @@
     <t>update information from SQL</t>
   </si>
   <si>
-    <t>sort procedures from price lowest to highest/vice versa</t>
-  </si>
-  <si>
     <t>so I can see results accurate to my budget</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t xml:space="preserve">I can easily use and navigate through the search features. </t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>I can search for any information I require from a single entity</t>
   </si>
   <si>
@@ -179,7 +173,7 @@
     <t>User story</t>
   </si>
   <si>
-    <t>In progress</t>
+    <t>sort procedures from price lowest to highest</t>
   </si>
 </sst>
 </file>
@@ -230,7 +224,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,12 +240,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF00FFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
@@ -280,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -298,13 +286,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,8 +300,8 @@
   <colors>
     <mruColors>
       <color rgb="FF00FFFF"/>
+      <color rgb="FF00FF00"/>
       <color rgb="FF00CCFF"/>
-      <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -534,7 +520,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -544,8 +530,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>48</v>
+      <c r="A1" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -758,7 +744,7 @@
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -811,10 +797,10 @@
         <v>18</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>32</v>
       </c>
       <c r="E11" s="10">
         <v>6</v>
@@ -837,10 +823,10 @@
         <v>18</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="E12" s="9">
         <v>3</v>
@@ -877,7 +863,7 @@
       <c r="G13" s="9">
         <v>1</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I13" s="9"/>
@@ -890,10 +876,10 @@
         <v>18</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E14" s="9">
         <v>8</v>
@@ -904,7 +890,7 @@
       <c r="G14" s="9">
         <v>2</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>10</v>
       </c>
       <c r="I14" s="9"/>
@@ -917,10 +903,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="E15" s="9">
         <v>9</v>
@@ -931,7 +917,7 @@
       <c r="G15" s="9">
         <v>2</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="12" t="s">
         <v>10</v>
       </c>
       <c r="I15" s="9"/>
@@ -944,10 +930,10 @@
         <v>18</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="E16" s="10">
         <v>6</v>
@@ -958,7 +944,7 @@
       <c r="G16" s="10">
         <v>2</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -970,10 +956,10 @@
         <v>18</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="E17" s="10">
         <v>6</v>
@@ -984,85 +970,85 @@
       <c r="G17" s="10">
         <v>2</v>
       </c>
-      <c r="H17" s="11" t="s">
-        <v>49</v>
+      <c r="H17" s="12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G18" s="6">
         <v>2</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>43</v>
+      <c r="H18" s="12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E19" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F19" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G19" s="6">
         <v>2</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>43</v>
+      <c r="H19" s="12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E20" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G20" s="9">
         <v>2</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1074,10 +1060,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="E21" s="9">
         <v>4</v>
@@ -1101,7 +1087,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
     <sortCondition ref="H20"/>
   </sortState>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>